<commit_message>
Chapter 3: Comparing Decomposition Implementations - Supervisor suggestions
Remove unnecessarily detailed text. Reuse important information from the Bandwidth section in the Speedup section and remove the rest.
</commit_message>
<xml_diff>
--- a/resources/plot-csv-files/14-matrices-double-precision-rci.xlsx
+++ b/resources/plot-csv-files/14-matrices-double-precision-rci.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cejkaluk\git\research-assignment-LU-decomposition\resources\plot-csv-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9378F5FD-2DA6-4D4A-90D5-B1B72E94E2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF2000C-5276-4257-938F-A54F933D92EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EB188C0A-FAF6-472A-8029-F7F1C455370D}"/>
   </bookViews>
@@ -36,24 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>id</t>
   </si>
   <si>
     <t>matrix-name</t>
-  </si>
-  <si>
-    <t>cm-bandwidth</t>
-  </si>
-  <si>
-    <t>icm8-bandwidth</t>
-  </si>
-  <si>
-    <t>icm16-bandwidth</t>
-  </si>
-  <si>
-    <t>icm32-bandwidth</t>
   </si>
   <si>
     <t>icm8-speedup</t>
@@ -459,26 +447,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EB636D-FE6B-437A-94AD-9719587C6509}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="C1" sqref="C1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,475 +471,295 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>1.9830000000000001</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0.187</v>
+        <v>9.4E-2</v>
       </c>
       <c r="E2">
-        <v>0.19</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="F2">
-        <v>0.186</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
         <v>9.4E-2</v>
       </c>
-      <c r="I2">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="J2">
-        <v>9.4E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0.32600000000000001</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>1.157</v>
+        <v>3.544</v>
       </c>
       <c r="E3">
-        <v>1.401</v>
+        <v>4.2949999999999999</v>
       </c>
       <c r="F3">
-        <v>1.196</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>3.544</v>
-      </c>
-      <c r="I3">
-        <v>4.2949999999999999</v>
-      </c>
-      <c r="J3">
         <v>3.6640000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>5.8000000000000003E-2</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>1.2250000000000001</v>
+        <v>21.192</v>
       </c>
       <c r="E4">
-        <v>0.52400000000000002</v>
+        <v>9.0619999999999994</v>
       </c>
       <c r="F4">
-        <v>0.41099999999999998</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>21.192</v>
-      </c>
-      <c r="I4">
-        <v>9.0619999999999994</v>
-      </c>
-      <c r="J4">
         <v>7.117</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>4.7E-2</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>7.0000000000000007E-2</v>
+        <v>1.5029999999999999</v>
       </c>
       <c r="E5">
-        <v>8.8999999999999996E-2</v>
+        <v>1.897</v>
       </c>
       <c r="F5">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1.5029999999999999</v>
-      </c>
-      <c r="I5">
-        <v>1.897</v>
-      </c>
-      <c r="J5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>1.6E-2</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>0.35599999999999998</v>
+        <v>22.553000000000001</v>
       </c>
       <c r="E6">
-        <v>0.44900000000000001</v>
+        <v>28.433</v>
       </c>
       <c r="F6">
-        <v>0.49299999999999999</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>22.553000000000001</v>
-      </c>
-      <c r="I6">
-        <v>28.433</v>
-      </c>
-      <c r="J6">
         <v>31.213999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C7">
-        <v>1.6E-2</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>2.3210000000000002</v>
+        <v>147.33799999999999</v>
       </c>
       <c r="E7">
-        <v>2.7370000000000001</v>
+        <v>173.756</v>
       </c>
       <c r="F7">
-        <v>3.4039999999999999</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>147.33799999999999</v>
-      </c>
-      <c r="I7">
-        <v>173.756</v>
-      </c>
-      <c r="J7">
         <v>216.11799999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>1.6E-2</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>3.0990000000000002</v>
+        <v>199.83099999999999</v>
       </c>
       <c r="E8">
-        <v>3.83</v>
+        <v>246.97</v>
       </c>
       <c r="F8">
-        <v>4.4550000000000001</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>199.83099999999999</v>
-      </c>
-      <c r="I8">
-        <v>246.97</v>
-      </c>
-      <c r="J8">
         <v>287.21800000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>1.4999999999999999E-2</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>11.377000000000001</v>
+        <v>767.23599999999999</v>
       </c>
       <c r="E9">
-        <v>14.291</v>
+        <v>963.79</v>
       </c>
       <c r="F9">
-        <v>16.873999999999999</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>767.23599999999999</v>
-      </c>
-      <c r="I9">
-        <v>963.79</v>
-      </c>
-      <c r="J9">
         <v>1137.979</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C10">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>8.82</v>
+        <v>435.75099999999998</v>
       </c>
       <c r="E10">
-        <v>9.968</v>
+        <v>492.50299999999999</v>
       </c>
       <c r="F10">
-        <v>10.945</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>435.75099999999998</v>
-      </c>
-      <c r="I10">
-        <v>492.50299999999999</v>
-      </c>
-      <c r="J10">
         <v>540.76</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C11">
-        <v>1.4E-2</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>0.02</v>
+        <v>1.476</v>
       </c>
       <c r="E11">
-        <v>2.5000000000000001E-2</v>
+        <v>1.859</v>
       </c>
       <c r="F11">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>1.476</v>
-      </c>
-      <c r="I11">
-        <v>1.859</v>
-      </c>
-      <c r="J11">
         <v>2.3490000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C12">
-        <v>1.4999999999999999E-2</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>2.3639999999999999</v>
+        <v>160.58000000000001</v>
       </c>
       <c r="E12">
-        <v>2.9540000000000002</v>
+        <v>200.67</v>
       </c>
       <c r="F12">
-        <v>3.625</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>160.58000000000001</v>
-      </c>
-      <c r="I12">
-        <v>200.67</v>
-      </c>
-      <c r="J12">
         <v>246.25800000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C13">
-        <v>1.4E-2</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>1.2999999999999999E-2</v>
+        <v>0.92300000000000004</v>
       </c>
       <c r="E13">
-        <v>1.7000000000000001E-2</v>
+        <v>1.149</v>
       </c>
       <c r="F13">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="I13">
-        <v>1.149</v>
-      </c>
-      <c r="J13">
         <v>1.4810000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C14">
-        <v>7.0000000000000001E-3</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>5.0549999999999997</v>
+        <v>766.851</v>
       </c>
       <c r="E14">
-        <v>6.7370000000000001</v>
+        <v>1022.014</v>
       </c>
       <c r="F14">
-        <v>8.8170000000000002</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>766.851</v>
-      </c>
-      <c r="I14">
-        <v>1022.014</v>
-      </c>
-      <c r="J14">
         <v>1337.5340000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C15">
-        <v>7.0000000000000001E-3</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>6.0000000000000001E-3</v>
+        <v>0.95599999999999996</v>
       </c>
       <c r="E15">
-        <v>8.0000000000000002E-3</v>
+        <v>1.2589999999999999</v>
       </c>
       <c r="F15">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>0.95599999999999996</v>
-      </c>
-      <c r="I15">
-        <v>1.2589999999999999</v>
-      </c>
-      <c r="J15">
         <v>1.67</v>
       </c>
     </row>

</xml_diff>